<commit_message>
Update filter and view
</commit_message>
<xml_diff>
--- a/query juni.xlsx
+++ b/query juni.xlsx
@@ -14,6 +14,9 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$Y$1:$Y$1202</definedName>
+  </definedNames>
   <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -5810,8 +5813,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AC1202"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Y1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="U1" sqref="U1:U1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5819,6 +5822,9 @@
     <col min="6" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.140625" customWidth="1"/>
+    <col min="14" max="14" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="34.5703125" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="22.85546875" customWidth="1"/>
     <col min="29" max="29" width="27.140625" bestFit="1" customWidth="1"/>
   </cols>
@@ -104625,6 +104631,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="Y1:Y1202" xr:uid="{2D244B93-319F-4DA3-903D-45B92795E888}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>